<commit_message>
Worked on analytic solution for experimental boundary conditions and comparing with experimental data
</commit_message>
<xml_diff>
--- a/data/DopantUptake/DopantUptake/QCMSummary.xlsx
+++ b/data/DopantUptake/DopantUptake/QCMSummary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\Diffusion-Modeling\data\DopantUptake\DopantUptake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC602F85-CCEC-472C-8D81-0617FBC05F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5385FB97-5EDB-4FE7-A8B7-A57A9AD5F9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8592662-5262-40EC-A6D9-6432A0CF2B82}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8592662-5262-40EC-A6D9-6432A0CF2B82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Thicknesses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Sample #</t>
   </si>
@@ -159,6 +160,12 @@
   </si>
   <si>
     <t>Doped Pi-Pi g</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Thickness [A]</t>
   </si>
 </sst>
 </file>
@@ -543,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D69824-7156-409E-8C82-126A0E9E05BE}">
   <dimension ref="A1:AG18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2341,4 +2348,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB8D9B5-5CF0-41C8-8A13-0EFA632C9E18}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>205.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>237.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>282.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>304.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>290.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>234.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>321.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>81</v>
+      </c>
+      <c r="B11">
+        <v>265.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>471.33332999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>441.33332999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>447.33332999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>375.66667000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>